<commit_message>
DOM Changes in PROD1
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/Prod/ALL_PAGES/END_TO_END/TC6_SearchResults_Typeahead.xlsx
+++ b/Input_files/Actual_testcases/Kaman/Prod/ALL_PAGES/END_TO_END/TC6_SearchResults_Typeahead.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Actual_testcases\Kaman\Prod\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73FAB0EC-AF0F-4CAC-90BE-4F94CFD61AD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5676CFF3-CC7E-45B6-9BD2-1DC78B7584D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC6_SearchResults_Typeahead" sheetId="1" r:id="rId1"/>
@@ -71,9 +71,6 @@
     <t>PRESS_ENTER</t>
   </si>
   <si>
-    <t>ValidSearchHeader</t>
-  </si>
-  <si>
     <t>validSearchV</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>Showing Results for "sprocket"</t>
+  </si>
+  <si>
+    <t>ValidSearchHeader1</t>
   </si>
 </sst>
 </file>
@@ -513,8 +513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -545,7 +545,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
@@ -565,7 +565,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>12</v>
@@ -580,7 +580,7 @@
         <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>14</v>
@@ -595,23 +595,23 @@
         <v>9</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -625,7 +625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -648,7 +648,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -669,7 +669,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="3" t="b">
         <v>1</v>
@@ -677,15 +677,15 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="3" t="b">
         <v>1</v>

</xml_diff>